<commit_message>
add excelgrep, rename the other scripts to excelxxx
</commit_message>
<xml_diff>
--- a/tbl.xlsx
+++ b/tbl.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael.moser\mystuff\datahelp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55C5144C-8681-47DC-83EF-55E6F82F02E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5D17F8-CE7D-4158-A1C3-DCF129CB34ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6940A38C-F402-4723-AEE8-8D6763920186}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{6940A38C-F402-4723-AEE8-8D6763920186}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>a col</t>
   </si>
@@ -63,6 +64,9 @@
   </si>
   <si>
     <t>g</t>
+  </si>
+  <si>
+    <t>e col</t>
   </si>
 </sst>
 </file>
@@ -436,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CFDD56D-3782-470D-9317-8AF701F9AA60}">
   <dimension ref="B4:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -500,4 +504,24 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9143A9F0-3935-4E25-97A9-2D4707220E65}">
+  <dimension ref="B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>